<commit_message>
sattled the keywords problems
</commit_message>
<xml_diff>
--- a/Title.xlsx
+++ b/Title.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ACCEPT_METHOD</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>CONTRACTENDDATE</t>
+  </si>
+  <si>
+    <t>AGENCY_NAME</t>
+  </si>
+  <si>
+    <t>SALE_COMPANY_NAME_FEE</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -619,6 +625,16 @@
         <v>28</v>
       </c>
     </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>